<commit_message>
Correct values for Monocytes in Buteo buteo inserted
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MOMO\Documents\01-PhD\01-Paper\13- Blood Chemistry\BloodChemistryR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A61BB3-5B25-4B08-AC37-CD62ECE147BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2323BB67-3719-4893-BF71-746FD1306658}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -390,10 +390,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -419,9 +425,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -704,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AD2" sqref="AD2"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39:L89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4097,7 +4104,7 @@
       <c r="K39">
         <v>12</v>
       </c>
-      <c r="L39">
+      <c r="L39" s="2">
         <v>2</v>
       </c>
       <c r="M39">
@@ -4191,8 +4198,8 @@
       <c r="K40">
         <v>12</v>
       </c>
-      <c r="L40">
-        <v>2</v>
+      <c r="L40" s="2">
+        <v>1</v>
       </c>
       <c r="M40">
         <v>54</v>
@@ -4285,8 +4292,8 @@
       <c r="K41">
         <v>30</v>
       </c>
-      <c r="L41">
-        <v>2</v>
+      <c r="L41" s="2">
+        <v>1</v>
       </c>
       <c r="M41">
         <v>42</v>
@@ -4379,8 +4386,8 @@
       <c r="K42">
         <v>23</v>
       </c>
-      <c r="L42">
-        <v>2</v>
+      <c r="L42" s="2">
+        <v>0</v>
       </c>
       <c r="M42">
         <v>30</v>
@@ -4470,8 +4477,8 @@
       <c r="K43">
         <v>24</v>
       </c>
-      <c r="L43">
-        <v>2</v>
+      <c r="L43" s="2">
+        <v>5</v>
       </c>
       <c r="M43">
         <v>39</v>
@@ -4564,8 +4571,8 @@
       <c r="K44">
         <v>35</v>
       </c>
-      <c r="L44">
-        <v>2</v>
+      <c r="L44" s="2">
+        <v>5</v>
       </c>
       <c r="M44">
         <v>40</v>
@@ -4652,7 +4659,7 @@
       <c r="K45">
         <v>16</v>
       </c>
-      <c r="L45">
+      <c r="L45" s="2">
         <v>2</v>
       </c>
       <c r="M45">
@@ -4740,8 +4747,8 @@
       <c r="K46">
         <v>16</v>
       </c>
-      <c r="L46">
-        <v>2</v>
+      <c r="L46" s="2">
+        <v>1</v>
       </c>
       <c r="M46">
         <v>35</v>
@@ -4834,8 +4841,8 @@
       <c r="K47">
         <v>13</v>
       </c>
-      <c r="L47">
-        <v>2</v>
+      <c r="L47" s="2">
+        <v>1</v>
       </c>
       <c r="M47">
         <v>55</v>
@@ -4928,8 +4935,8 @@
       <c r="K48">
         <v>12</v>
       </c>
-      <c r="L48">
-        <v>2</v>
+      <c r="L48" s="2">
+        <v>1</v>
       </c>
       <c r="M48">
         <v>38</v>
@@ -5019,8 +5026,8 @@
       <c r="K49">
         <v>16</v>
       </c>
-      <c r="L49">
-        <v>2</v>
+      <c r="L49" s="2">
+        <v>8</v>
       </c>
       <c r="M49">
         <v>37</v>
@@ -5107,8 +5114,8 @@
       <c r="K50">
         <v>43</v>
       </c>
-      <c r="L50">
-        <v>2</v>
+      <c r="L50" s="2">
+        <v>5</v>
       </c>
       <c r="M50">
         <v>28</v>
@@ -5201,8 +5208,8 @@
       <c r="K51">
         <v>29</v>
       </c>
-      <c r="L51">
-        <v>2</v>
+      <c r="L51" s="2">
+        <v>3</v>
       </c>
       <c r="M51">
         <v>33</v>
@@ -5295,8 +5302,8 @@
       <c r="K52">
         <v>12</v>
       </c>
-      <c r="L52">
-        <v>2</v>
+      <c r="L52" s="2">
+        <v>1</v>
       </c>
       <c r="M52">
         <v>45</v>
@@ -5389,8 +5396,8 @@
       <c r="K53">
         <v>21</v>
       </c>
-      <c r="L53">
-        <v>2</v>
+      <c r="L53" s="2">
+        <v>3</v>
       </c>
       <c r="M53">
         <v>33</v>
@@ -5483,8 +5490,8 @@
       <c r="K54">
         <v>28</v>
       </c>
-      <c r="L54">
-        <v>2</v>
+      <c r="L54" s="2">
+        <v>1</v>
       </c>
       <c r="M54">
         <v>26</v>
@@ -5571,8 +5578,8 @@
       <c r="K55">
         <v>25</v>
       </c>
-      <c r="L55">
-        <v>2</v>
+      <c r="L55" s="2">
+        <v>1</v>
       </c>
       <c r="M55">
         <v>34</v>
@@ -5665,8 +5672,8 @@
       <c r="K56">
         <v>22</v>
       </c>
-      <c r="L56">
-        <v>2</v>
+      <c r="L56" s="2">
+        <v>0</v>
       </c>
       <c r="M56">
         <v>25</v>
@@ -5753,8 +5760,8 @@
       <c r="K57">
         <v>25</v>
       </c>
-      <c r="L57">
-        <v>2</v>
+      <c r="L57" s="2">
+        <v>0</v>
       </c>
       <c r="M57">
         <v>30</v>
@@ -5841,8 +5848,8 @@
       <c r="K58">
         <v>26</v>
       </c>
-      <c r="L58">
-        <v>2</v>
+      <c r="L58" s="2">
+        <v>1</v>
       </c>
       <c r="M58">
         <v>41</v>
@@ -5929,8 +5936,8 @@
       <c r="K59">
         <v>12</v>
       </c>
-      <c r="L59">
-        <v>2</v>
+      <c r="L59" s="2">
+        <v>0</v>
       </c>
       <c r="M59">
         <v>56</v>
@@ -6023,8 +6030,8 @@
       <c r="K60">
         <v>16</v>
       </c>
-      <c r="L60">
-        <v>2</v>
+      <c r="L60" s="2">
+        <v>1</v>
       </c>
       <c r="M60">
         <v>38</v>
@@ -6117,8 +6124,8 @@
       <c r="K61">
         <v>24</v>
       </c>
-      <c r="L61">
-        <v>2</v>
+      <c r="L61" s="2">
+        <v>3</v>
       </c>
       <c r="M61">
         <v>30</v>
@@ -6211,8 +6218,8 @@
       <c r="K62">
         <v>19</v>
       </c>
-      <c r="L62">
-        <v>2</v>
+      <c r="L62" s="2">
+        <v>3</v>
       </c>
       <c r="M62">
         <v>32</v>
@@ -6299,8 +6306,8 @@
       <c r="K63">
         <v>16</v>
       </c>
-      <c r="L63">
-        <v>2</v>
+      <c r="L63" s="2">
+        <v>4</v>
       </c>
       <c r="M63">
         <v>28</v>
@@ -6387,8 +6394,8 @@
       <c r="K64">
         <v>25</v>
       </c>
-      <c r="L64">
-        <v>2</v>
+      <c r="L64" s="2">
+        <v>3</v>
       </c>
       <c r="M64">
         <v>22</v>
@@ -6481,8 +6488,8 @@
       <c r="K65">
         <v>18</v>
       </c>
-      <c r="L65">
-        <v>2</v>
+      <c r="L65" s="2">
+        <v>4</v>
       </c>
       <c r="M65">
         <v>38</v>
@@ -6569,8 +6576,8 @@
       <c r="K66">
         <v>21</v>
       </c>
-      <c r="L66">
-        <v>2</v>
+      <c r="L66" s="2">
+        <v>6</v>
       </c>
       <c r="M66">
         <v>38</v>
@@ -6663,7 +6670,7 @@
       <c r="K67">
         <v>20</v>
       </c>
-      <c r="L67">
+      <c r="L67" s="2">
         <v>2</v>
       </c>
       <c r="M67">
@@ -6751,8 +6758,8 @@
       <c r="K68">
         <v>48</v>
       </c>
-      <c r="L68">
-        <v>2</v>
+      <c r="L68" s="2">
+        <v>4</v>
       </c>
       <c r="M68">
         <v>45</v>
@@ -6839,8 +6846,8 @@
       <c r="K69">
         <v>26</v>
       </c>
-      <c r="L69">
-        <v>2</v>
+      <c r="L69" s="2">
+        <v>6</v>
       </c>
       <c r="M69">
         <v>25</v>
@@ -6927,8 +6934,8 @@
       <c r="K70">
         <v>71</v>
       </c>
-      <c r="L70">
-        <v>2</v>
+      <c r="L70" s="2">
+        <v>3</v>
       </c>
       <c r="M70">
         <v>17</v>
@@ -7015,8 +7022,8 @@
       <c r="K71">
         <v>30</v>
       </c>
-      <c r="L71">
-        <v>2</v>
+      <c r="L71" s="2">
+        <v>4</v>
       </c>
       <c r="M71">
         <v>30</v>
@@ -7103,8 +7110,8 @@
       <c r="K72">
         <v>38</v>
       </c>
-      <c r="L72">
-        <v>2</v>
+      <c r="L72" s="2">
+        <v>4</v>
       </c>
       <c r="M72">
         <v>26</v>
@@ -7197,8 +7204,8 @@
       <c r="K73">
         <v>34</v>
       </c>
-      <c r="L73">
-        <v>2</v>
+      <c r="L73" s="2">
+        <v>4</v>
       </c>
       <c r="M73">
         <v>18</v>
@@ -7285,7 +7292,7 @@
       <c r="K74">
         <v>45</v>
       </c>
-      <c r="L74">
+      <c r="L74" s="2">
         <v>2</v>
       </c>
       <c r="M74">
@@ -7373,8 +7380,8 @@
       <c r="K75">
         <v>22</v>
       </c>
-      <c r="L75">
-        <v>2</v>
+      <c r="L75" s="2">
+        <v>4</v>
       </c>
       <c r="M75">
         <v>39</v>
@@ -7461,8 +7468,8 @@
       <c r="K76">
         <v>46</v>
       </c>
-      <c r="L76">
-        <v>2</v>
+      <c r="L76" s="2">
+        <v>1</v>
       </c>
       <c r="M76">
         <v>50</v>
@@ -7555,8 +7562,8 @@
       <c r="K77">
         <v>36</v>
       </c>
-      <c r="L77">
-        <v>2</v>
+      <c r="L77" s="2">
+        <v>1</v>
       </c>
       <c r="M77">
         <v>36</v>
@@ -7643,7 +7650,7 @@
       <c r="K78">
         <v>17</v>
       </c>
-      <c r="L78">
+      <c r="L78" s="2">
         <v>2</v>
       </c>
       <c r="M78">
@@ -7731,8 +7738,8 @@
       <c r="K79">
         <v>19</v>
       </c>
-      <c r="L79">
-        <v>2</v>
+      <c r="L79" s="2">
+        <v>3</v>
       </c>
       <c r="M79">
         <v>39</v>
@@ -7825,7 +7832,7 @@
       <c r="K80">
         <v>23</v>
       </c>
-      <c r="L80">
+      <c r="L80" s="2">
         <v>2</v>
       </c>
       <c r="M80">
@@ -7913,7 +7920,7 @@
       <c r="K81">
         <v>32</v>
       </c>
-      <c r="L81">
+      <c r="L81" s="2">
         <v>2</v>
       </c>
       <c r="M81">
@@ -8007,8 +8014,8 @@
       <c r="K82">
         <v>18</v>
       </c>
-      <c r="L82">
-        <v>2</v>
+      <c r="L82" s="2">
+        <v>7</v>
       </c>
       <c r="M82">
         <v>34</v>
@@ -8098,8 +8105,8 @@
       <c r="K83">
         <v>32</v>
       </c>
-      <c r="L83">
-        <v>2</v>
+      <c r="L83" s="2">
+        <v>4</v>
       </c>
       <c r="M83">
         <v>33</v>
@@ -8192,8 +8199,8 @@
       <c r="K84">
         <v>23</v>
       </c>
-      <c r="L84">
-        <v>2</v>
+      <c r="L84" s="2">
+        <v>6</v>
       </c>
       <c r="M84">
         <v>27</v>
@@ -8280,8 +8287,8 @@
       <c r="K85">
         <v>20</v>
       </c>
-      <c r="L85">
-        <v>2</v>
+      <c r="L85" s="2">
+        <v>7</v>
       </c>
       <c r="M85">
         <v>27</v>
@@ -8374,8 +8381,8 @@
       <c r="K86">
         <v>26</v>
       </c>
-      <c r="L86">
-        <v>2</v>
+      <c r="L86" s="2">
+        <v>1</v>
       </c>
       <c r="M86">
         <v>48</v>
@@ -8468,8 +8475,8 @@
       <c r="K87">
         <v>39</v>
       </c>
-      <c r="L87">
-        <v>2</v>
+      <c r="L87" s="2">
+        <v>3</v>
       </c>
       <c r="M87">
         <v>25</v>
@@ -8556,8 +8563,8 @@
       <c r="K88">
         <v>31</v>
       </c>
-      <c r="L88">
-        <v>2</v>
+      <c r="L88" s="2">
+        <v>3</v>
       </c>
       <c r="M88">
         <v>26</v>
@@ -8647,8 +8654,8 @@
       <c r="K89">
         <v>33</v>
       </c>
-      <c r="L89">
-        <v>2</v>
+      <c r="L89" s="2">
+        <v>4</v>
       </c>
       <c r="M89">
         <v>37</v>

</xml_diff>

<commit_message>
inserted correct Morphs of buzzards
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MOMO\Documents\01-PhD\01-Paper\13- Blood Chemistry\BloodChemistryR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2323BB67-3719-4893-BF71-746FD1306658}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5397205-2169-4F7D-A039-2B21B036A56F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -711,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39:L89"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4284,7 +4284,7 @@
         <v>0.54388641441758256</v>
       </c>
       <c r="I41">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J41">
         <v>12400</v>
@@ -4378,7 +4378,7 @@
         <v>0.53279166397802202</v>
       </c>
       <c r="I42">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J42">
         <v>7600</v>
@@ -4563,7 +4563,7 @@
         <v>0.49653129353846176</v>
       </c>
       <c r="I44">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J44">
         <v>8400</v>
@@ -4651,7 +4651,7 @@
         <v>0.50910571428571416</v>
       </c>
       <c r="I45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J45">
         <v>16000</v>
@@ -4739,7 +4739,7 @@
         <v>0.53059912087912109</v>
       </c>
       <c r="I46">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J46">
         <v>16000</v>
@@ -4833,7 +4833,7 @@
         <v>0.41420568826373622</v>
       </c>
       <c r="I47">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J47">
         <v>16000</v>
@@ -4927,7 +4927,7 @@
         <v>0.60567574013186776</v>
       </c>
       <c r="I48">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J48">
         <v>17200</v>
@@ -5106,7 +5106,7 @@
         <v>0.50489094540659341</v>
       </c>
       <c r="I50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J50">
         <v>13600</v>
@@ -5199,9 +5199,6 @@
         <f t="shared" si="5"/>
         <v>0.42265631859340658</v>
       </c>
-      <c r="I51">
-        <v>3</v>
-      </c>
       <c r="J51">
         <v>12800</v>
       </c>
@@ -5294,7 +5291,7 @@
         <v>0.50489094540659341</v>
       </c>
       <c r="I52">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J52">
         <v>17600</v>
@@ -5570,7 +5567,7 @@
         <v>0.67228451320879101</v>
       </c>
       <c r="I55">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J55">
         <v>9200</v>
@@ -5664,7 +5661,7 @@
         <v>0.65839867287912102</v>
       </c>
       <c r="I56">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J56">
         <v>10000</v>
@@ -5752,7 +5749,7 @@
         <v>0.59816543628571417</v>
       </c>
       <c r="I57">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J57">
         <v>6800</v>
@@ -6116,7 +6113,7 @@
         <v>0.46372278364835168</v>
       </c>
       <c r="I61">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J61">
         <v>10800</v>
@@ -6210,7 +6207,7 @@
         <v>0.52191128826373645</v>
       </c>
       <c r="I62">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J62">
         <v>24000</v>
@@ -6386,7 +6383,7 @@
         <v>0.59075828430769228</v>
       </c>
       <c r="I64">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J64">
         <v>20000</v>
@@ -6662,7 +6659,7 @@
         <v>0.42265631859340658</v>
       </c>
       <c r="I67">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J67">
         <v>18800</v>
@@ -7014,7 +7011,7 @@
         <v>0.45558602057142855</v>
       </c>
       <c r="I71">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J71">
         <v>13400</v>
@@ -7102,7 +7099,7 @@
         <v>0.61328998626373643</v>
       </c>
       <c r="I72">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J72">
         <v>28000</v>
@@ -7196,7 +7193,7 @@
         <v>0.65839867287912102</v>
       </c>
       <c r="I73">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J73">
         <v>16400</v>
@@ -7372,7 +7369,7 @@
         <v>0.44129705826373639</v>
       </c>
       <c r="I75">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J75">
         <v>16000</v>
@@ -7460,7 +7457,7 @@
         <v>0.59321593826373631</v>
       </c>
       <c r="I76">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J76">
         <v>9200</v>
@@ -7642,7 +7639,7 @@
         <v>0.48413709749450556</v>
       </c>
       <c r="I78">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J78">
         <v>8000</v>
@@ -7730,7 +7727,7 @@
         <v>0.59321593826373631</v>
       </c>
       <c r="I79">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J79">
         <v>8000</v>
@@ -7824,7 +7821,7 @@
         <v>0.56445811813186819</v>
       </c>
       <c r="I80">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J80">
         <v>8400</v>
@@ -7912,7 +7909,7 @@
         <v>0.52841499057142849</v>
       </c>
       <c r="I81">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J81">
         <v>12000</v>
@@ -8006,7 +8003,7 @@
         <v>0.59568497441758217</v>
       </c>
       <c r="I82">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J82">
         <v>13600</v>
@@ -8279,7 +8276,7 @@
         <v>0.54838884782417563</v>
       </c>
       <c r="I85">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J85">
         <v>17200</v>
@@ -8373,7 +8370,7 @@
         <v>0.6807441758241759</v>
       </c>
       <c r="I86">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J86">
         <v>16800</v>
@@ -8467,7 +8464,7 @@
         <v>0.77286748287912066</v>
       </c>
       <c r="I87">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J87">
         <v>22000</v>
@@ -8555,7 +8552,7 @@
         <v>0.82252120771428572</v>
       </c>
       <c r="I88">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J88">
         <v>13200</v>
@@ -8646,7 +8643,7 @@
         <v>0.58345310925274751</v>
       </c>
       <c r="I89">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J89">
         <v>13600</v>

</xml_diff>